<commit_message>
Criação de relacionamento entre parceiro e nc
</commit_message>
<xml_diff>
--- a/src/assets/files/exemplo_setor.xlsx
+++ b/src/assets/files/exemplo_setor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A23D6C4-262E-44AC-B039-633B4CED4CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB86087D-15DA-4A3A-82B6-747CC73A423F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6750" yWindow="750" windowWidth="21600" windowHeight="13590" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$J$418</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$418</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,36 +28,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>F000006</t>
+    <t>nome_responsavel</t>
   </si>
   <si>
-    <t>F000011</t>
+    <t>email_responsavel</t>
   </si>
   <si>
-    <t>F000013</t>
+    <t>telefone_responsavel</t>
   </si>
   <si>
-    <t>F000015</t>
-  </si>
-  <si>
-    <t>F000025</t>
-  </si>
-  <si>
-    <t>F000027</t>
-  </si>
-  <si>
-    <t>F000029</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>codigo_pn</t>
+    <t>nome</t>
   </si>
 </sst>
 </file>
@@ -425,77 +407,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="41.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="1019" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:D418" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mudança no excel de setores e siglas no dashboard
</commit_message>
<xml_diff>
--- a/src/assets/files/exemplo_setor.xlsx
+++ b/src/assets/files/exemplo_setor.xlsx
@@ -10,20 +10,17 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$J$418</definedName>
-  </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -36,6 +33,9 @@
   <si>
     <t xml:space="preserve">telefone_responsável</t>
   </si>
+  <si>
+    <t xml:space="preserve">siglas</t>
+  </si>
 </sst>
 </file>
 
@@ -44,11 +44,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -68,26 +67,25 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,11 +127,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,68 +147,50 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="41.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.41"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:J418"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>